<commit_message>
Agregamos reseñas de las areas en la base de datos
</commit_message>
<xml_diff>
--- a/Source/AnalisisExploratorioANP/Estadísticas ANPs RMBA.xlsx
+++ b/Source/AnalisisExploratorioANP/Estadísticas ANPs RMBA.xlsx
@@ -25,7 +25,9 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ANPs!$A$1:$M$48</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Partidos!$A$1:$K$45</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ANPs!$A$1:$M$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ANPs!$A$1:$M$48</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Partidos!$A$1:$K$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Partidos!$A$1:$K$45</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -444,7 +446,7 @@
     <t xml:space="preserve">Lavallol</t>
   </si>
   <si>
-    <t xml:space="preserve">Fue creada en el año 2011 con la finalidad de conservar la biodiversidad y los valores históricos y promover la educación ambiental.</t>
+    <t xml:space="preserve">Fue creada en el año 1991 con la finalidad de promover la educación ambiental.</t>
   </si>
   <si>
     <t xml:space="preserve">Reserva Natural Municipal Vicente Lopez</t>
@@ -540,6 +542,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Fue creada alrededor del año 2000 como</t>
     </r>
@@ -549,6 +552,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -558,6 +562,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">espacio de recreación y esparcimiento.</t>
     </r>
@@ -584,6 +589,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Fue creada en el año 1991 para la</t>
     </r>
@@ -593,6 +599,7 @@
         <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -602,6 +609,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">protección de pajonales y de la comunidad ribereña. Además, posee importancia ornitológica debido a la presencia de una población residente y nidificante de la pajonalera pico recto.</t>
     </r>
@@ -843,12 +851,13 @@
     <numFmt numFmtId="167" formatCode="0%"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -871,12 +880,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -885,10 +889,25 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Arial"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -901,6 +920,11 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1013,7 +1037,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1054,11 +1078,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1066,7 +1094,7 @@
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1087,10 +1115,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1134,10 +1158,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1148,10 +1168,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1197,10 +1213,10 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF98B855"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF4F81BD"/>
       <rgbColor rgb="FF9BBB59"/>
@@ -1212,7 +1228,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFDC853E"/>
       <rgbColor rgb="FF4672A8"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF558ED5"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1223,24 +1239,24 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00B0F0"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF558ED5"/>
+      <rgbColor rgb="FF83CAFF"/>
       <rgbColor rgb="FFD09493"/>
       <rgbColor rgb="FF8064A2"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF98B855"/>
       <rgbColor rgb="FF4A7EBB"/>
       <rgbColor rgb="FF4BACC6"/>
-      <rgbColor rgb="FF92D050"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFAECF00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF725990"/>
       <rgbColor rgb="FF8AA64F"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF4299B0"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF314004"/>
       <rgbColor rgb="FFC0504D"/>
       <rgbColor rgb="FFBE4B48"/>
       <rgbColor rgb="FF7D5FA0"/>
@@ -1621,11 +1637,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="97869963"/>
-        <c:axId val="30490679"/>
+        <c:axId val="19770555"/>
+        <c:axId val="23247427"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97869963"/>
+        <c:axId val="19770555"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,14 +1677,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30490679"/>
+        <c:crossAx val="23247427"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30490679"/>
+        <c:axId val="23247427"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1730,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97869963"/>
+        <c:crossAx val="19770555"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2616,12 +2632,12 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="80831580"/>
-        <c:axId val="5289747"/>
+        <c:axId val="73097657"/>
+        <c:axId val="89162690"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="80831580"/>
+        <c:axId val="73097657"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2657,14 +2673,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5289747"/>
+        <c:crossAx val="89162690"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5289747"/>
+        <c:axId val="89162690"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2710,7 +2726,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80831580"/>
+        <c:crossAx val="73097657"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3284,11 +3300,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="8508853"/>
-        <c:axId val="54756867"/>
+        <c:axId val="29940755"/>
+        <c:axId val="58441821"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8508853"/>
+        <c:axId val="29940755"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,14 +3340,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54756867"/>
+        <c:crossAx val="58441821"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54756867"/>
+        <c:axId val="58441821"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3377,7 +3393,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8508853"/>
+        <c:crossAx val="29940755"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3500,11 +3516,11 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="81525571"/>
-        <c:axId val="2438496"/>
+        <c:axId val="7822929"/>
+        <c:axId val="62003928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81525571"/>
+        <c:axId val="7822929"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3540,14 +3556,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2438496"/>
+        <c:crossAx val="62003928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2438496"/>
+        <c:axId val="62003928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3583,7 +3599,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81525571"/>
+        <c:crossAx val="7822929"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3968,10 +3984,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0775663942798774"/>
-          <c:y val="0.0514435695538058"/>
-          <c:w val="0.726953524004086"/>
-          <c:h val="0.83254593175853"/>
+          <c:x val="0.0775713464853476"/>
+          <c:y val="0.0514503215645098"/>
+          <c:w val="0.726936091425653"/>
+          <c:h val="0.83239270245439"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4140,11 +4156,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="58983229"/>
-        <c:axId val="37000305"/>
+        <c:axId val="92842842"/>
+        <c:axId val="32052326"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58983229"/>
+        <c:axId val="92842842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4180,14 +4196,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37000305"/>
+        <c:crossAx val="32052326"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37000305"/>
+        <c:axId val="32052326"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4233,7 +4249,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58983229"/>
+        <c:crossAx val="92842842"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4605,11 +4621,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="23110927"/>
-        <c:axId val="35095911"/>
+        <c:axId val="16278808"/>
+        <c:axId val="21301033"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23110927"/>
+        <c:axId val="16278808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4645,14 +4661,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35095911"/>
+        <c:crossAx val="21301033"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35095911"/>
+        <c:axId val="21301033"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4698,7 +4714,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23110927"/>
+        <c:crossAx val="16278808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4780,8 +4796,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.325418039410704"/>
-          <c:y val="0.0374704180909808"/>
+          <c:x val="0.325519214028106"/>
+          <c:y val="0.0377284080452215"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5031,11 +5047,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="19260644"/>
-        <c:axId val="55498815"/>
+        <c:axId val="55642209"/>
+        <c:axId val="41399600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="19260644"/>
+        <c:axId val="55642209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5071,14 +5087,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55498815"/>
+        <c:crossAx val="41399600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55498815"/>
+        <c:axId val="41399600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5124,7 +5140,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19260644"/>
+        <c:crossAx val="55642209"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5333,11 +5349,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="68280968"/>
-        <c:axId val="198348"/>
+        <c:axId val="41014054"/>
+        <c:axId val="99040157"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68280968"/>
+        <c:axId val="41014054"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5373,14 +5389,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198348"/>
+        <c:crossAx val="99040157"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198348"/>
+        <c:axId val="99040157"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5426,7 +5442,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68280968"/>
+        <c:crossAx val="41014054"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5798,11 +5814,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="66553241"/>
-        <c:axId val="88556961"/>
+        <c:axId val="91683024"/>
+        <c:axId val="92252804"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66553241"/>
+        <c:axId val="91683024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5838,14 +5854,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88556961"/>
+        <c:crossAx val="92252804"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88556961"/>
+        <c:axId val="92252804"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5891,7 +5907,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66553241"/>
+        <c:crossAx val="91683024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6004,6 +6020,24 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -6051,11 +6085,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="80591537"/>
-        <c:axId val="52687050"/>
+        <c:axId val="1117246"/>
+        <c:axId val="2919832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80591537"/>
+        <c:axId val="1117246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6091,14 +6125,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52687050"/>
+        <c:crossAx val="2919832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52687050"/>
+        <c:axId val="2919832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6144,7 +6178,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80591537"/>
+        <c:crossAx val="1117246"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6785,11 +6819,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="24275432"/>
-        <c:axId val="19421443"/>
+        <c:axId val="55977931"/>
+        <c:axId val="51334803"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="24275432"/>
+        <c:axId val="55977931"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6825,14 +6859,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19421443"/>
+        <c:crossAx val="51334803"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19421443"/>
+        <c:axId val="51334803"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6878,7 +6912,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24275432"/>
+        <c:crossAx val="55977931"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6967,7 +7001,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"Superficie ANPs en la RMBA"</c:f>
+              <c:f>label 0</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7036,21 +7070,21 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Partidos!$D$1;Partidos!$F$1</c:f>
+              <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Superficie RMBA (ha.)</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Superficie ANP (ha.)</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Partidos!$D$43;Partidos!$F$43</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -7958,12 +7992,12 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="68034348"/>
-        <c:axId val="57399073"/>
+        <c:axId val="53364010"/>
+        <c:axId val="7712099"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="68034348"/>
+        <c:axId val="53364010"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7999,14 +8033,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57399073"/>
+        <c:crossAx val="7712099"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57399073"/>
+        <c:axId val="7712099"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8052,7 +8086,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68034348"/>
+        <c:crossAx val="53364010"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8166,6 +8200,78 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -8249,11 +8355,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="42043800"/>
-        <c:axId val="72456425"/>
+        <c:axId val="33909182"/>
+        <c:axId val="94673377"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42043800"/>
+        <c:axId val="33909182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8289,14 +8395,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72456425"/>
+        <c:crossAx val="94673377"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72456425"/>
+        <c:axId val="94673377"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8342,7 +8448,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42043800"/>
+        <c:crossAx val="33909182"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8394,9 +8500,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8405,7 +8511,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3601800" y="190440"/>
-        <a:ext cx="5789520" cy="2738520"/>
+        <a:ext cx="5789160" cy="2738160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8424,9 +8530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>456840</xdr:colOff>
+      <xdr:colOff>456480</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8435,7 +8541,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3962160" y="3292200"/>
-        <a:ext cx="5638680" cy="2741760"/>
+        <a:ext cx="5638320" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8459,9 +8565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>390240</xdr:colOff>
+      <xdr:colOff>389880</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8470,7 +8576,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3449160" y="190440"/>
-        <a:ext cx="3989520" cy="2285640"/>
+        <a:ext cx="3989160" cy="2285280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8489,9 +8595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>395640</xdr:colOff>
+      <xdr:colOff>395280</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8500,7 +8606,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3335040" y="2842920"/>
-        <a:ext cx="5632920" cy="2742840"/>
+        <a:ext cx="5632560" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8524,9 +8630,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>571320</xdr:colOff>
+      <xdr:colOff>570960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8534,8 +8640,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5324400" y="1139400"/>
-        <a:ext cx="5638680" cy="3123000"/>
+        <a:off x="5352840" y="1139400"/>
+        <a:ext cx="5638320" cy="3122640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8559,9 +8665,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>571320</xdr:colOff>
+      <xdr:colOff>570960</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8570,7 +8676,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="76320" y="133200"/>
-        <a:ext cx="16497000" cy="4590720"/>
+        <a:ext cx="16496640" cy="4590360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8594,9 +8700,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>195840</xdr:colOff>
+      <xdr:colOff>195480</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8604,8 +8710,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9763200" y="2120400"/>
-        <a:ext cx="5891400" cy="2743200"/>
+        <a:off x="9810720" y="2120400"/>
+        <a:ext cx="5900760" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8624,9 +8730,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>381600</xdr:colOff>
+      <xdr:colOff>381240</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8634,8 +8740,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2562120" y="10249920"/>
-        <a:ext cx="10992240" cy="3560760"/>
+        <a:off x="2581200" y="10249920"/>
+        <a:ext cx="11030040" cy="3560400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8654,9 +8760,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>239040</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8664,8 +8770,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9848880" y="5406480"/>
-        <a:ext cx="6611400" cy="3328560"/>
+        <a:off x="9896400" y="5406480"/>
+        <a:ext cx="6620760" cy="3328200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8689,9 +8795,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>343440</xdr:colOff>
+      <xdr:colOff>343080</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8700,7 +8806,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5992560" y="538200"/>
-        <a:ext cx="6028200" cy="3461760"/>
+        <a:ext cx="6027840" cy="3461400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8724,9 +8830,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>400680</xdr:colOff>
+      <xdr:colOff>400320</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8734,8 +8840,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4335120" y="119160"/>
-        <a:ext cx="6828480" cy="3528720"/>
+        <a:off x="4344840" y="119160"/>
+        <a:ext cx="6828120" cy="3528360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8754,9 +8860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257040</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8764,8 +8870,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9802440" y="1395360"/>
-        <a:ext cx="5789880" cy="2743560"/>
+        <a:off x="9812160" y="1395360"/>
+        <a:ext cx="5789520" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8789,9 +8895,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>309960</xdr:colOff>
+      <xdr:colOff>309600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8799,8 +8905,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4095720" y="185760"/>
-        <a:ext cx="5643720" cy="2742840"/>
+        <a:off x="4114800" y="185760"/>
+        <a:ext cx="5643360" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8819,9 +8925,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8829,8 +8935,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10220040" y="233280"/>
-        <a:ext cx="5638680" cy="2743560"/>
+        <a:off x="10239120" y="233280"/>
+        <a:ext cx="5638320" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8849,9 +8955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257040</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8859,8 +8965,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10753560" y="3310920"/>
-        <a:ext cx="5791320" cy="2741760"/>
+        <a:off x="10772640" y="3310920"/>
+        <a:ext cx="5790960" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8879,9 +8985,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
+      <xdr:colOff>46800</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8890,7 +8996,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="828720" y="4724280"/>
-        <a:ext cx="7124040" cy="3005280"/>
+        <a:ext cx="7142760" cy="3004920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8909,9 +9015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>209880</xdr:colOff>
+      <xdr:colOff>209520</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8919,8 +9025,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8420040" y="7502040"/>
-        <a:ext cx="5791320" cy="2742120"/>
+        <a:off x="8439120" y="7502040"/>
+        <a:ext cx="5790960" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8944,9 +9050,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8955,7 +9061,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1001160" y="1929960"/>
-        <a:ext cx="5389560" cy="2741760"/>
+        <a:ext cx="5398560" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8974,9 +9080,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>276120</xdr:colOff>
+      <xdr:colOff>275760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8984,8 +9090,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7926120" y="739440"/>
-        <a:ext cx="5284800" cy="2741760"/>
+        <a:off x="7935840" y="739440"/>
+        <a:ext cx="5284080" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9009,9 +9115,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>495000</xdr:colOff>
+      <xdr:colOff>494640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>167040</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9020,7 +9126,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4000320" y="280800"/>
-        <a:ext cx="5638680" cy="2743560"/>
+        <a:ext cx="5638320" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9039,9 +9145,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9050,7 +9156,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3838320" y="3433680"/>
-        <a:ext cx="5638680" cy="2742840"/>
+        <a:ext cx="5638320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9074,9 +9180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>161280</xdr:colOff>
+      <xdr:colOff>160920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9085,7 +9191,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2829960" y="81000"/>
-        <a:ext cx="5789520" cy="2742840"/>
+        <a:ext cx="5789160" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9104,9 +9210,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>295560</xdr:colOff>
+      <xdr:colOff>295200</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9115,7 +9221,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3724200" y="3168360"/>
-        <a:ext cx="5791320" cy="2741760"/>
+        <a:ext cx="5790960" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9135,28 +9241,28 @@
   </sheetPr>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="K39" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
-      <selection pane="topRight" activeCell="N47" activeCellId="0" sqref="N47"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="I33" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topRight" activeCell="N35" activeCellId="0" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.6396761133603"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="45.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="46.2753036437247"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="true" max="16" min="16" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
@@ -10656,7 +10762,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="n">
         <v>34</v>
       </c>
@@ -10696,7 +10802,7 @@
       <c r="M35" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N35" s="7" t="s">
+      <c r="N35" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -10872,7 +10978,7 @@
       <c r="M39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N39" s="10" t="s">
+      <c r="N39" s="11" t="s">
         <v>149</v>
       </c>
     </row>
@@ -10883,7 +10989,7 @@
       <c r="B40" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C40" s="11" t="n">
+      <c r="C40" s="12" t="n">
         <v>1200</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -10916,7 +11022,7 @@
       <c r="M40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N40" s="12" t="s">
+      <c r="N40" s="13" t="s">
         <v>153</v>
       </c>
     </row>
@@ -10960,7 +11066,7 @@
       <c r="M41" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N41" s="12" t="s">
+      <c r="N41" s="13" t="s">
         <v>157</v>
       </c>
     </row>
@@ -11048,7 +11154,7 @@
       <c r="M43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N43" s="13" t="s">
+      <c r="N43" s="14" t="s">
         <v>165</v>
       </c>
     </row>
@@ -11136,7 +11242,7 @@
       <c r="M45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N45" s="12" t="s">
+      <c r="N45" s="13" t="s">
         <v>171</v>
       </c>
     </row>
@@ -11180,7 +11286,7 @@
       <c r="M46" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N46" s="12" t="s">
+      <c r="N46" s="13" t="s">
         <v>174</v>
       </c>
     </row>
@@ -11229,7 +11335,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="14" t="n">
+      <c r="C48" s="15" t="n">
         <f aca="false">SUM(C41:C46,C2:C39)</f>
         <v>186484</v>
       </c>
@@ -11297,13 +11403,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>227</v>
       </c>
     </row>
@@ -11402,21 +11508,21 @@
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="13" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="36" t="n">
+      <c r="B2" s="34" t="n">
         <f aca="false">COUNTIF(ANPs!M2:M46, "Si")</f>
         <v>28</v>
       </c>
@@ -11440,13 +11546,13 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>227</v>
       </c>
     </row>
@@ -11539,16 +11645,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -11577,7 +11683,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="35" t="s">
         <v>234</v>
       </c>
       <c r="B5" s="5" t="n">
@@ -11585,7 +11691,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="35" t="s">
         <v>235</v>
       </c>
       <c r="B6" s="5" t="n">
@@ -11625,7 +11731,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="35" t="s">
         <v>240</v>
       </c>
       <c r="B11" s="5" t="n">
@@ -11657,16 +11763,16 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="38" t="n">
+      <c r="B15" s="36" t="n">
         <f aca="false">SUM(B2:B14)</f>
         <v>3858.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>244</v>
       </c>
       <c r="B17" s="20" t="n">
@@ -11675,7 +11781,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>245</v>
       </c>
       <c r="B18" s="20" t="n">
@@ -11684,10 +11790,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="B19" s="40" t="n">
+      <c r="B19" s="38" t="n">
         <f aca="false">(B15*100)/B17</f>
         <v>2.06907831234851</v>
       </c>
@@ -11745,37 +11851,37 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>183</v>
       </c>
     </row>
@@ -11799,7 +11905,7 @@
       <c r="F2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="18" t="n">
+      <c r="G2" s="19" t="n">
         <f aca="false">(F2*100)/D2</f>
         <v>0</v>
       </c>
@@ -11821,17 +11927,17 @@
       <c r="E3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="19" t="n">
+      <c r="F3" s="5" t="n">
         <v>152</v>
       </c>
-      <c r="G3" s="18" t="n">
+      <c r="G3" s="19" t="n">
         <f aca="false">(F3*100)/D3</f>
         <v>2.89965661961084</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="17" t="s">
         <v>186</v>
       </c>
     </row>
@@ -11852,10 +11958,10 @@
       <c r="E4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="F4" s="5" t="n">
         <v>8200</v>
       </c>
-      <c r="G4" s="18" t="n">
+      <c r="G4" s="19" t="n">
         <f aca="false">(F4*100)/D4</f>
         <v>43.6170212765957</v>
       </c>
@@ -11883,10 +11989,10 @@
       <c r="E5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="19" t="n">
+      <c r="F5" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="G5" s="18" t="n">
+      <c r="G5" s="19" t="n">
         <f aca="false">(F5*100)/D5</f>
         <v>11.1111111111111</v>
       </c>
@@ -11914,10 +12020,10 @@
       <c r="E6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="18" t="n">
+      <c r="G6" s="19" t="n">
         <f aca="false">(F6*100)/D6</f>
         <v>0</v>
       </c>
@@ -11945,10 +12051,10 @@
       <c r="E7" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="F7" s="5" t="n">
         <v>5455</v>
       </c>
-      <c r="G7" s="18" t="n">
+      <c r="G7" s="19" t="n">
         <f aca="false">(F7*100)/D7</f>
         <v>6.11547085201794</v>
       </c>
@@ -11976,10 +12082,10 @@
       <c r="E8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="19" t="n">
+      <c r="F8" s="5" t="n">
         <v>129</v>
       </c>
-      <c r="G8" s="18" t="n">
+      <c r="G8" s="19" t="n">
         <f aca="false">(F8*100)/D8</f>
         <v>0.107231920199501</v>
       </c>
@@ -12008,10 +12114,10 @@
       <c r="E9" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="19" t="n">
+      <c r="F9" s="5" t="n">
         <v>424</v>
       </c>
-      <c r="G9" s="18" t="n">
+      <c r="G9" s="19" t="n">
         <f aca="false">(F9*100)/D9</f>
         <v>2.0855878012789</v>
       </c>
@@ -12033,10 +12139,10 @@
       <c r="E10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="19" t="n">
+      <c r="F10" s="5" t="n">
         <v>2200</v>
       </c>
-      <c r="G10" s="18" t="n">
+      <c r="G10" s="19" t="n">
         <f aca="false">(F10*100)/D10</f>
         <v>21.7821782178218</v>
       </c>
@@ -12058,10 +12164,10 @@
       <c r="E11" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="19" t="n">
+      <c r="F11" s="5" t="n">
         <v>99</v>
       </c>
-      <c r="G11" s="18" t="n">
+      <c r="G11" s="19" t="n">
         <f aca="false">(F11*100)/D11</f>
         <v>0.357400722021661</v>
       </c>
@@ -12083,10 +12189,10 @@
       <c r="E12" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="19" t="n">
+      <c r="F12" s="5" t="n">
         <v>630</v>
       </c>
-      <c r="G12" s="18" t="n">
+      <c r="G12" s="19" t="n">
         <f aca="false">(F12*100)/D12</f>
         <v>5.24039261354184</v>
       </c>
@@ -12108,10 +12214,10 @@
       <c r="E13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="19" t="n">
+      <c r="F13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="18" t="n">
+      <c r="G13" s="19" t="n">
         <f aca="false">(F13*100)/D13</f>
         <v>0</v>
       </c>
@@ -12133,10 +12239,10 @@
       <c r="E14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="19" t="n">
+      <c r="F14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="18" t="n">
+      <c r="G14" s="19" t="n">
         <f aca="false">(F14*100)/D14</f>
         <v>0</v>
       </c>
@@ -12158,10 +12264,10 @@
       <c r="E15" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="19" t="n">
+      <c r="F15" s="5" t="n">
         <v>254</v>
       </c>
-      <c r="G15" s="18" t="n">
+      <c r="G15" s="19" t="n">
         <f aca="false">(F15*100)/D15</f>
         <v>1.33684210526316</v>
       </c>
@@ -12186,7 +12292,7 @@
       <c r="F16" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="18" t="n">
+      <c r="G16" s="19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12207,10 +12313,10 @@
       <c r="E17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="19" t="n">
+      <c r="F17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="18" t="n">
+      <c r="G17" s="19" t="n">
         <f aca="false">(F17*100)/D17</f>
         <v>0</v>
       </c>
@@ -12232,10 +12338,10 @@
       <c r="E18" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="19" t="n">
+      <c r="F18" s="5" t="n">
         <v>34.8</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G18" s="19" t="n">
         <f aca="false">(F18*100)/D18</f>
         <v>0.982218458933107</v>
       </c>
@@ -12257,10 +12363,10 @@
       <c r="E19" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="19" t="n">
+      <c r="F19" s="5" t="n">
         <v>8.7</v>
       </c>
-      <c r="G19" s="18" t="n">
+      <c r="G19" s="19" t="n">
         <f aca="false">(F19*100)/D19</f>
         <v>0.227510460251046</v>
       </c>
@@ -12282,10 +12388,10 @@
       <c r="E20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="19" t="n">
+      <c r="F20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="18" t="n">
+      <c r="G20" s="19" t="n">
         <f aca="false">(F20*100)/D20</f>
         <v>0</v>
       </c>
@@ -12307,10 +12413,10 @@
       <c r="E21" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="19" t="n">
+      <c r="F21" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="G21" s="18" t="n">
+      <c r="G21" s="19" t="n">
         <f aca="false">(F21*100)/D21</f>
         <v>0.911244760342628</v>
       </c>
@@ -12332,10 +12438,10 @@
       <c r="E22" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="F22" s="19" t="n">
+      <c r="F22" s="5" t="n">
         <v>71401</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="19" t="n">
         <f aca="false">(F22*100)/D22</f>
         <v>77.1069114470842</v>
       </c>
@@ -12357,10 +12463,10 @@
       <c r="E23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="19" t="n">
+      <c r="F23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="18" t="n">
+      <c r="G23" s="19" t="n">
         <f aca="false">(F23*100)/D23</f>
         <v>0</v>
       </c>
@@ -12382,10 +12488,10 @@
       <c r="E24" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="19" t="n">
+      <c r="F24" s="5" t="n">
         <v>744.5</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="19" t="n">
         <f aca="false">(F24*100)/D24</f>
         <v>8.52806414662085</v>
       </c>
@@ -12407,10 +12513,10 @@
       <c r="E25" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="19" t="n">
+      <c r="F25" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="19" t="n">
         <f aca="false">(F25*100)/D25</f>
         <v>0.01875</v>
       </c>
@@ -12432,10 +12538,10 @@
       <c r="E26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="19" t="n">
+      <c r="F26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="19" t="n">
         <f aca="false">(F26*100)/D26</f>
         <v>0</v>
       </c>
@@ -12457,10 +12563,10 @@
       <c r="E27" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F27" s="19" t="n">
+      <c r="F27" s="5" t="n">
         <v>460</v>
       </c>
-      <c r="G27" s="18" t="n">
+      <c r="G27" s="19" t="n">
         <f aca="false">(F27*100)/D27</f>
         <v>0.978723404255319</v>
       </c>
@@ -12482,10 +12588,10 @@
       <c r="E28" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F28" s="19" t="n">
+      <c r="F28" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="18" t="n">
+      <c r="G28" s="19" t="n">
         <f aca="false">(F28*100)/D28</f>
         <v>0</v>
       </c>
@@ -12507,10 +12613,10 @@
       <c r="E29" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F29" s="19" t="n">
+      <c r="F29" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="G29" s="18" t="n">
+      <c r="G29" s="19" t="n">
         <f aca="false">(F29*100)/D29</f>
         <v>5.37258905066352</v>
       </c>
@@ -12532,10 +12638,10 @@
       <c r="E30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F30" s="19" t="n">
+      <c r="F30" s="5" t="n">
         <v>14.5</v>
       </c>
-      <c r="G30" s="18" t="n">
+      <c r="G30" s="19" t="n">
         <f aca="false">(F30*100)/D30</f>
         <v>0.260510240747395</v>
       </c>
@@ -12557,10 +12663,10 @@
       <c r="E31" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F31" s="19" t="n">
+      <c r="F31" s="5" t="n">
         <v>297</v>
       </c>
-      <c r="G31" s="18" t="n">
+      <c r="G31" s="19" t="n">
         <f aca="false">(F31*100)/D31</f>
         <v>0.84375</v>
       </c>
@@ -12585,7 +12691,7 @@
       <c r="F32" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="18" t="n">
+      <c r="G32" s="19" t="n">
         <f aca="false">(F32*100)/D32</f>
         <v>0</v>
       </c>
@@ -12610,7 +12716,7 @@
       <c r="F33" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="G33" s="18" t="n">
+      <c r="G33" s="19" t="n">
         <f aca="false">(F33*100)/D33</f>
         <v>1.63952344518527</v>
       </c>
@@ -12635,7 +12741,7 @@
       <c r="F34" s="5" t="n">
         <v>88624</v>
       </c>
-      <c r="G34" s="18" t="n">
+      <c r="G34" s="19" t="n">
         <f aca="false">(F34*100)/D34</f>
         <v>91.0832476875642</v>
       </c>
@@ -12660,7 +12766,7 @@
       <c r="F35" s="5" t="n">
         <v>55.5</v>
       </c>
-      <c r="G35" s="18" t="n">
+      <c r="G35" s="19" t="n">
         <f aca="false">(F35*100)/D35</f>
         <v>1.15625</v>
       </c>
@@ -12685,7 +12791,7 @@
       <c r="F36" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="19" t="n">
         <f aca="false">(F36*100)/D36</f>
         <v>0.392857142857143</v>
       </c>
@@ -12710,7 +12816,7 @@
       <c r="F37" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G37" s="18" t="n">
+      <c r="G37" s="19" t="n">
         <f aca="false">(F37*100)/D37</f>
         <v>0.0963855421686747</v>
       </c>
@@ -12735,7 +12841,7 @@
       <c r="F38" s="5" t="n">
         <v>132</v>
       </c>
-      <c r="G38" s="18" t="n">
+      <c r="G38" s="19" t="n">
         <f aca="false">(F38*100)/D38</f>
         <v>0.198198198198198</v>
       </c>
@@ -12760,7 +12866,7 @@
       <c r="F39" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G39" s="18" t="n">
+      <c r="G39" s="19" t="n">
         <f aca="false">(F39*100)/D39</f>
         <v>0.108695652173913</v>
       </c>
@@ -12785,7 +12891,7 @@
       <c r="F40" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="18" t="n">
+      <c r="G40" s="19" t="n">
         <f aca="false">(F40*100)/D40</f>
         <v>0</v>
       </c>
@@ -12810,7 +12916,7 @@
       <c r="F41" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G41" s="18" t="n">
+      <c r="G41" s="19" t="n">
         <f aca="false">(F41*100)/D41</f>
         <v>0.0769230769230769</v>
       </c>
@@ -12835,7 +12941,7 @@
       <c r="F42" s="5" t="n">
         <v>4131</v>
       </c>
-      <c r="G42" s="18" t="n">
+      <c r="G42" s="19" t="n">
         <f aca="false">(F42*100)/D42</f>
         <v>3.43677204658902</v>
       </c>
@@ -12897,10 +13003,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>212</v>
       </c>
     </row>
@@ -12965,20 +13071,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>213</v>
       </c>
     </row>
@@ -13047,7 +13153,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="24" t="s">
         <v>194</v>
       </c>
       <c r="B7" s="20" t="n">
@@ -13084,7 +13190,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -13205,39 +13311,39 @@
       <c r="C10" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="17" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>142</v>
       </c>
       <c r="B19" s="20" t="n">
@@ -13270,7 +13376,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B20" s="20" t="n">
@@ -13303,7 +13409,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="20" t="n">
@@ -13336,7 +13442,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="20" t="n">
@@ -13369,7 +13475,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="20" t="n">
@@ -13411,36 +13517,36 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="G44" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H44" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I44" s="16" t="s">
+      <c r="I44" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>142</v>
       </c>
       <c r="B45" s="20" t="n">
@@ -13469,7 +13575,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="20" t="n">
@@ -13498,7 +13604,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="20" t="n">
@@ -13527,7 +13633,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B48" s="20" t="n">
@@ -13556,7 +13662,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B49" s="20" t="n">
@@ -13619,20 +13725,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="F3" s="33" t="s">
+      <c r="D3" s="31"/>
+      <c r="F3" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="G3" s="33"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="20" t="s">
@@ -13683,7 +13789,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="29" t="s">
         <v>194</v>
       </c>
       <c r="D8" s="20" t="n">
@@ -13756,13 +13862,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>227</v>
       </c>
     </row>
@@ -13897,13 +14003,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>